<commit_message>
Updates to SQL and codebook to align changes from implementations
</commit_message>
<xml_diff>
--- a/tbemr_basicRegister_codebook_v1.3.xlsx
+++ b/tbemr_basicRegister_codebook_v1.3.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msfintl-my.sharepoint.com/personal/kristina_reinhardt_newyork_msf_org/Documents/github/mart-tbemr-query-library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3F628ECC-ADCD-4099-BEC7-9B7DA5B7586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A6D9B58-FB13-44C1-87C3-AF181C93877B}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{3F628ECC-ADCD-4099-BEC7-9B7DA5B7586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F6BF6C-BE2F-4B3B-A894-C17B5CB41E4B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="30" windowWidth="38640" windowHeight="15840" xr2:uid="{A005DB92-A8DC-40CC-A3FD-38C99E047FDE}"/>
+    <workbookView xWindow="14505" yWindow="-13500" windowWidth="12000" windowHeight="12900" xr2:uid="{A005DB92-A8DC-40CC-A3FD-38C99E047FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="query_changelog" sheetId="2" r:id="rId1"/>
     <sheet name="basic_register_description" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">basic_register_description!$A$1:$J$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">basic_register_description!$A$1:$J$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="313">
   <si>
     <t>Column</t>
   </si>
@@ -733,207 +733,9 @@
     <t>Renamed column names (added numbering) to adjust for Metabase automatic alphabetical ordering in v0.31 and v0.34</t>
   </si>
   <si>
-    <t>02_Register</t>
-  </si>
-  <si>
-    <t>01_Registration_Number</t>
-  </si>
-  <si>
-    <t>04_Sex</t>
-  </si>
-  <si>
-    <t>05_Age_at_Registration</t>
-  </si>
-  <si>
-    <t>07_WHO_Registration_Group</t>
-  </si>
-  <si>
-    <t>08_History_of_Previously_Treated</t>
-  </si>
-  <si>
-    <t>10_MTB_Confirmed</t>
-  </si>
-  <si>
-    <t>11_Drug_Resistance_Profile</t>
-  </si>
-  <si>
-    <t>12_Sub-class_of_Drug_Resistance_Profile</t>
-  </si>
-  <si>
-    <t>13_Treatment_Start_Date</t>
-  </si>
-  <si>
-    <t>14_Treatment_Duration_(months)</t>
-  </si>
-  <si>
-    <t>16_Start_Date_(Dlm)</t>
-  </si>
-  <si>
-    <t>17_Start_Date_(Bdq)</t>
-  </si>
-  <si>
-    <t>18_Start_Date_(Dlm_or_Bdq)</t>
-  </si>
-  <si>
-    <t>19_Start_Date_(Dlm_and_Bdq)</t>
-  </si>
-  <si>
-    <t>20_Last_Facility</t>
-  </si>
-  <si>
-    <t>46_HIV_Baseline</t>
-  </si>
-  <si>
-    <t>47_HIV_Lab</t>
-  </si>
-  <si>
-    <t>48_HIV_Status</t>
-  </si>
-  <si>
-    <t>49_Hep_B_Baseline</t>
-  </si>
-  <si>
-    <t>50_Hep_B_Lab</t>
-  </si>
-  <si>
-    <t>51_Hep_B_Status</t>
-  </si>
-  <si>
-    <t>52_Hep_C_Baseline</t>
-  </si>
-  <si>
-    <t>53_Hep_C_Lab</t>
-  </si>
-  <si>
-    <t>54_Hep_C_Status</t>
-  </si>
-  <si>
-    <t>55_Diabetes_Baseline</t>
-  </si>
-  <si>
-    <t>56_Positive_Culture_at_Baseline</t>
-  </si>
-  <si>
-    <t>58_Culture_Conversion_(for_positive_at_baseline_only)</t>
-  </si>
-  <si>
-    <t>59_Initial_Culture_Conversion_Date</t>
-  </si>
-  <si>
-    <t>60_Months_to_Initial_Culture_Conversion</t>
-  </si>
-  <si>
-    <t>62_Outcome</t>
-  </si>
-  <si>
-    <t>09_Baseline_Disease_Site</t>
-  </si>
-  <si>
-    <t>63_End_of_Treatment_Date</t>
-  </si>
-  <si>
-    <t>57_Negative_Culture_Closer_to_Baseline_Than_Positive_Culture</t>
-  </si>
-  <si>
-    <t>21_Initial_Drug_H</t>
-  </si>
-  <si>
-    <t>22_Initial_Drug_R</t>
-  </si>
-  <si>
-    <t>23_Initial_Drug_E</t>
-  </si>
-  <si>
-    <t>24_Initial_Drug_Z</t>
-  </si>
-  <si>
-    <t>25_Initial_Drug_S</t>
-  </si>
-  <si>
-    <t>26_Initial_Drug_Am</t>
-  </si>
-  <si>
-    <t>27_Initial_Drug_Km</t>
-  </si>
-  <si>
-    <t>28_Initial_Drug_Cm</t>
-  </si>
-  <si>
-    <t>29_Initial_Drug_Lfx</t>
-  </si>
-  <si>
-    <t>30_Initial_Drug_Mfx</t>
-  </si>
-  <si>
-    <t>31_Initial_Drug_Pto</t>
-  </si>
-  <si>
-    <t>32_Initial_Drug_Eto</t>
-  </si>
-  <si>
-    <t>33_Initial_Drug_Cs</t>
-  </si>
-  <si>
-    <t>34_Initial_Drug_Trd</t>
-  </si>
-  <si>
-    <t>35_Initial_Drug_PAS</t>
-  </si>
-  <si>
-    <t>36_Initial_Drug_PAS-Na</t>
-  </si>
-  <si>
-    <t>37_Initial_Drug_Bdq</t>
-  </si>
-  <si>
-    <t>38_Initial_Drug_Dlm</t>
-  </si>
-  <si>
-    <t>39_Initial_Drug_Lzd</t>
-  </si>
-  <si>
-    <t>40_Initial_Drug_Cfz</t>
-  </si>
-  <si>
-    <t>41_Initial_Drug_Imp/Clm</t>
-  </si>
-  <si>
-    <t>42_Initial_Drug_Amx/Clv</t>
-  </si>
-  <si>
-    <t>43_Initial_Drug_Mpm</t>
-  </si>
-  <si>
-    <t>44_Initial_Drug_Pa</t>
-  </si>
-  <si>
-    <t>45_Initial_Drug_Rpt_or_P</t>
-  </si>
-  <si>
-    <t>06_Age_Group_at_Registration</t>
-  </si>
-  <si>
-    <t>03_EMR_ID</t>
-  </si>
-  <si>
-    <t>64_Next_Visit</t>
-  </si>
-  <si>
-    <t>61_Reconversion_after_Initial_Culture_Conversion</t>
-  </si>
-  <si>
-    <t>15_Second_Line_Treatment_Type</t>
-  </si>
-  <si>
     <t>Modified for use of patient_program_id instead of patient_id + program_id. Added background columns for summing/counting in metabase.</t>
   </si>
   <si>
-    <t>65_background_sum</t>
-  </si>
-  <si>
-    <t>64_background_count</t>
-  </si>
-  <si>
     <t>This is a background column to allow for more simple summing in Metabase</t>
   </si>
   <si>
@@ -947,6 +749,266 @@
   </si>
   <si>
     <t>Removed voided program enrollements</t>
+  </si>
+  <si>
+    <t>Add patient_id and patient_program_id columns to register to faciltate.
+Removed column name numbering to facilitate future changes to query. Number should not longer be needed in Metabase with Admin ability to clean table appearance and column order.
+Harmonization of query version with main query (all implementations to be on v1.6 of register)</t>
+  </si>
+  <si>
+    <t>Registration_Number</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>EMR_ID</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Age_at_Registration</t>
+  </si>
+  <si>
+    <t>Age_Group_at_Registration</t>
+  </si>
+  <si>
+    <t>WHO_Registration_Group</t>
+  </si>
+  <si>
+    <t>History_of_Previously_Treated</t>
+  </si>
+  <si>
+    <t>Baseline_Disease_Site</t>
+  </si>
+  <si>
+    <t>MTB_Confirmed</t>
+  </si>
+  <si>
+    <t>Drug_Resistance_Profile</t>
+  </si>
+  <si>
+    <t>Sub-class_of_Drug_Resistance_Profile</t>
+  </si>
+  <si>
+    <t>Treatment_Start_Date</t>
+  </si>
+  <si>
+    <t>This is the MDRTB start year from the treatment initiation form</t>
+  </si>
+  <si>
+    <t>This is the MDRTB start quarter + year from the treatment initiation form</t>
+  </si>
+  <si>
+    <t>Treatment_Start_Year</t>
+  </si>
+  <si>
+    <t>Treatment_Start_Quarter</t>
+  </si>
+  <si>
+    <t>Treatment_Duration_(months)</t>
+  </si>
+  <si>
+    <t>Second_Line_Treatment_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The date the patient baseline assessment took place. </t>
+  </si>
+  <si>
+    <t>Baseline form &gt; Date of Baseline</t>
+  </si>
+  <si>
+    <t>Date of Baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The year the patient baseline assessment took place. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The year and quarter the patient baseline assessment took place. </t>
+  </si>
+  <si>
+    <t>Clinic_Enrollment_Date</t>
+  </si>
+  <si>
+    <t>Clinic_Enrollment_Year</t>
+  </si>
+  <si>
+    <t>Clinic_Enrollment_Quarter</t>
+  </si>
+  <si>
+    <t>Start_Date_(Dlm)</t>
+  </si>
+  <si>
+    <t>Start_Date_(Bdq)</t>
+  </si>
+  <si>
+    <t>Start_Date_(Dlm_or_Bdq)</t>
+  </si>
+  <si>
+    <t>Start_Date_(Dlm_and_Bdq)</t>
+  </si>
+  <si>
+    <t>Last_Facility</t>
+  </si>
+  <si>
+    <t>Initial_Drug_H</t>
+  </si>
+  <si>
+    <t>Initial_Drug_R</t>
+  </si>
+  <si>
+    <t>Initial_Drug_E</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Z</t>
+  </si>
+  <si>
+    <t>Initial_Drug_S</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Am</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Km</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Cm</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Lfx</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Mfx</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Pto</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Eto</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Cs</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Trd</t>
+  </si>
+  <si>
+    <t>Initial_Drug_PAS</t>
+  </si>
+  <si>
+    <t>Initial_Drug_PAS-Na</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Bdq</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Dlm</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Lzd</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Cfz</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Imp/Clm</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Amx/Clv</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Mpm</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Pa</t>
+  </si>
+  <si>
+    <t>Initial_Drug_Rpt_or_P</t>
+  </si>
+  <si>
+    <t>HIV_Baseline</t>
+  </si>
+  <si>
+    <t>HIV_Lab</t>
+  </si>
+  <si>
+    <t>HIV_Status</t>
+  </si>
+  <si>
+    <t>Hep_B_Baseline</t>
+  </si>
+  <si>
+    <t>Hep_B_Lab</t>
+  </si>
+  <si>
+    <t>Hep_B_Status</t>
+  </si>
+  <si>
+    <t>Hep_C_Baseline</t>
+  </si>
+  <si>
+    <t>Hep_C_Lab</t>
+  </si>
+  <si>
+    <t>Hep_C_Status</t>
+  </si>
+  <si>
+    <t>Diabetes_Baseline</t>
+  </si>
+  <si>
+    <t>Positive_Culture_at_Baseline</t>
+  </si>
+  <si>
+    <t>Negative_Culture_Closer_to_Baseline_Than_Positive_Culture</t>
+  </si>
+  <si>
+    <t>Culture_Conversion_(for_positive_at_baseline_only)</t>
+  </si>
+  <si>
+    <t>Initial_Culture_Conversion_Date</t>
+  </si>
+  <si>
+    <t>Months_to_Initial_Culture_Conversion</t>
+  </si>
+  <si>
+    <t>Reconversion_after_Initial_Culture_Conversion</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>End_of_Treatment_Date</t>
+  </si>
+  <si>
+    <t>Next_Visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The patient_id is a background id number assigned in the OMRS database to identify data associated with a particular patient. This column can be used to connect data from other tables available in the analytics database with this register for further analysis in the tool. This column should be used when connecting additional demographic data to this register. Demographic data includes any data collected in the registration page of Bahmni. </t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The patient_program_id is a background id number assigned in the OMRS database to identify data associated with a particular patient program enrollment. This column can be used to connect data from other tables available in the analytics database with this register for further analysis in the tool. This column should be used when connecting additional data during care to this register. Additional data includes any data collected in the clinical module in Bahmni. </t>
+  </si>
+  <si>
+    <t>patient_program_id</t>
+  </si>
+  <si>
+    <t>patietn_program_id</t>
+  </si>
+  <si>
+    <t>background_sum</t>
+  </si>
+  <si>
+    <t>background_count</t>
   </si>
 </sst>
 </file>
@@ -1242,12 +1304,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1274,13 +1336,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1627,7 +1686,7 @@
   <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1640,24 +1699,24 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>43521</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1771,49 +1830,55 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="2:4" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>44169</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>285</v>
+        <v>221</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="19">
         <v>44834</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-    </row>
-    <row r="17" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-    </row>
-    <row r="18" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-    </row>
-    <row r="19" spans="2:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="2:4" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="19">
+        <v>44966</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
@@ -1829,61 +1894,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755CC844-63E2-4B85-BD9F-12E3C1EFFCA3}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46" style="11" customWidth="1"/>
-    <col min="2" max="2" width="33" style="11" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" style="11" customWidth="1"/>
-    <col min="4" max="6" width="27" style="11" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="11" customWidth="1"/>
-    <col min="8" max="9" width="23" style="11" customWidth="1"/>
-    <col min="10" max="10" width="49.109375" style="11" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="11"/>
+    <col min="1" max="1" width="46" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="27" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="23" style="1" customWidth="1"/>
+    <col min="10" max="10" width="49.109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="13" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" s="12" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="42" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -1907,12 +1972,12 @@
         <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -1944,7 +2009,7 @@
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>281</v>
+        <v>230</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
@@ -1973,7 +2038,7 @@
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -2005,7 +2070,7 @@
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>32</v>
@@ -2034,7 +2099,7 @@
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>280</v>
+        <v>233</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>35</v>
@@ -2063,7 +2128,7 @@
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>161</v>
@@ -2092,7 +2157,7 @@
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>162</v>
@@ -2121,7 +2186,7 @@
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>164</v>
@@ -2150,7 +2215,7 @@
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>165</v>
@@ -2179,7 +2244,7 @@
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>163</v>
@@ -2208,7 +2273,7 @@
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>166</v>
@@ -2237,7 +2302,7 @@
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>167</v>
@@ -2264,114 +2329,114 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>190</v>
+        <v>58</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>284</v>
+        <v>244</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>169</v>
+        <v>242</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>158</v>
+        <v>57</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>175</v>
+        <v>61</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>247</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>248</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>65</v>
+        <v>249</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>58</v>
@@ -2379,25 +2444,22 @@
       <c r="H18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>146</v>
+        <v>250</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>248</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>65</v>
+        <v>249</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>14</v>
@@ -2408,25 +2470,22 @@
       <c r="H19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>148</v>
+        <v>251</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>248</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>65</v>
+        <v>249</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>14</v>
@@ -2437,25 +2496,22 @@
       <c r="H20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:10" s="2" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>204</v>
+        <v>56</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>205</v>
+        <v>158</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>14</v>
@@ -2464,77 +2520,68 @@
         <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>209</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
@@ -2542,95 +2589,89 @@
         <v>257</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>75</v>
+        <v>148</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="2" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>259</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>16</v>
+        <v>205</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>72</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
@@ -2638,7 +2679,7 @@
         <v>260</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>70</v>
@@ -2650,7 +2691,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>209</v>
+        <v>14</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>15</v>
@@ -2670,7 +2711,7 @@
         <v>261</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>70</v>
@@ -2702,7 +2743,7 @@
         <v>262</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>70</v>
@@ -2734,7 +2775,7 @@
         <v>263</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>70</v>
@@ -2766,7 +2807,7 @@
         <v>264</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>70</v>
@@ -2798,7 +2839,7 @@
         <v>265</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>70</v>
@@ -2830,7 +2871,7 @@
         <v>266</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>70</v>
@@ -2862,7 +2903,7 @@
         <v>267</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>70</v>
@@ -2894,7 +2935,7 @@
         <v>268</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>70</v>
@@ -2926,7 +2967,7 @@
         <v>269</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>70</v>
@@ -2958,7 +2999,7 @@
         <v>270</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>70</v>
@@ -2990,7 +3031,7 @@
         <v>271</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>70</v>
@@ -3022,7 +3063,7 @@
         <v>272</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>70</v>
@@ -3054,7 +3095,7 @@
         <v>273</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>70</v>
@@ -3086,7 +3127,7 @@
         <v>274</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>70</v>
@@ -3118,7 +3159,7 @@
         <v>275</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>70</v>
@@ -3150,7 +3191,7 @@
         <v>276</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>70</v>
@@ -3182,7 +3223,7 @@
         <v>277</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>70</v>
@@ -3214,7 +3255,7 @@
         <v>278</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>208</v>
+        <v>90</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>70</v>
@@ -3246,7 +3287,7 @@
         <v>279</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>207</v>
+        <v>91</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>70</v>
@@ -3273,358 +3314,367 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>237</v>
+        <v>280</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="2" t="s">
+      <c r="F52" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B48" s="2" t="s">
+      <c r="I52" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="2" t="s">
+      <c r="F53" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J53" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B49" s="2" t="s">
+    <row r="54" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H49" s="2" t="s">
+      <c r="F54" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>103</v>
       </c>
       <c r="J54" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" s="2" t="s">
+    <row r="57" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I55" s="2" t="s">
+      <c r="E57" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I57" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J55" s="2" t="s">
+      <c r="J57" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="2" t="s">
+    <row r="58" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="E58" s="2" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>209</v>
@@ -3633,27 +3683,27 @@
         <v>15</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>191</v>
+        <v>97</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>248</v>
+        <v>292</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>218</v>
+        <v>122</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>195</v>
+        <v>123</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>197</v>
+        <v>100</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>199</v>
+        <v>124</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>209</v>
@@ -3662,85 +3712,91 @@
         <v>15</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>217</v>
+        <v>114</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>216</v>
+        <v>103</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>249</v>
+        <v>293</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>192</v>
+        <v>125</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>209</v>
@@ -3751,25 +3807,25 @@
       <c r="H62" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="J62" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>251</v>
+        <v>296</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>174</v>
+        <v>215</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>131</v>
+        <v>197</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>132</v>
+        <v>199</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>209</v>
@@ -3778,56 +3834,56 @@
         <v>15</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>133</v>
+        <v>191</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>253</v>
+        <v>297</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>131</v>
+        <v>197</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>136</v>
+        <v>199</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>209</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>16</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>138</v>
+        <v>195</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>209</v>
@@ -3839,56 +3895,53 @@
         <v>16</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="2" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>288</v>
+        <v>193</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>16</v>
+        <v>197</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>16</v>
+        <v>199</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>209</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H66" s="2">
-        <v>1</v>
+        <v>190</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>16</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>289</v>
+        <v>194</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>16</v>
+        <v>196</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>16</v>
+        <v>198</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>209</v>
@@ -3897,14 +3950,220 @@
         <v>15</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>290</v>
+        <v>191</v>
       </c>
       <c r="I67" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="2" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" s="2" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" s="2" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H73" s="2">
+        <v>1</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I74" s="2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J65" xr:uid="{F3A09C70-F2B3-4544-AF29-19179100C3E5}"/>
+  <autoFilter ref="A1:J70" xr:uid="{F3A09C70-F2B3-4544-AF29-19179100C3E5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>